<commit_message>
implementación de patrón facade para simplificar uso de servicios
</commit_message>
<xml_diff>
--- a/documentacion/2. Planeación/5. Estimación por puntos de función.xlsx
+++ b/documentacion/2. Planeación/5. Estimación por puntos de función.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="19485" yWindow="465" windowWidth="18915" windowHeight="21060" tabRatio="500"/>
+    <workbookView xWindow="19485" yWindow="465" windowWidth="18915" windowHeight="21060" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Resumen" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="166">
   <si>
     <t>Identificación del Proyecto</t>
   </si>
@@ -518,6 +518,24 @@
   </si>
   <si>
     <t>Campos (id, nombre)</t>
+  </si>
+  <si>
+    <t>Correo restablecimiento de contraseña</t>
+  </si>
+  <si>
+    <t>Correo notificación reserva realizada</t>
+  </si>
+  <si>
+    <t>Correo notificación reserva cancelada</t>
+  </si>
+  <si>
+    <t>Correo notificación reserva cancelada por administrador</t>
+  </si>
+  <si>
+    <t>DETs (token), FTR (tabla de tokens)</t>
+  </si>
+  <si>
+    <t>DETs (tipo, nombre, dia, inicio, fin), FTRs (tabla reservas)</t>
   </si>
 </sst>
 </file>
@@ -727,24 +745,36 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -775,6 +805,15 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -804,27 +843,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1108,7 +1126,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
@@ -1121,45 +1139,45 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="25" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="27"/>
+      <c r="A1" s="28" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="29"/>
+      <c r="C1" s="30"/>
     </row>
     <row r="2" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="30" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="31"/>
-      <c r="C2" s="32"/>
+      <c r="A2" s="34" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="35"/>
+      <c r="C2" s="36"/>
     </row>
     <row r="3" spans="1:6" ht="104.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="28" t="s">
+      <c r="B3" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="29"/>
+      <c r="C3" s="33"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="23" t="s">
+      <c r="B4" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="23"/>
+      <c r="C4" s="26"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="24">
+      <c r="B5" s="27">
         <v>42781</v>
       </c>
-      <c r="C5" s="24"/>
+      <c r="C5" s="27"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="17"/>
@@ -1167,11 +1185,11 @@
       <c r="C6" s="18"/>
     </row>
     <row r="7" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A7" s="22" t="s">
+      <c r="A7" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="22"/>
-      <c r="C7" s="22"/>
+      <c r="B7" s="31"/>
+      <c r="C7" s="31"/>
       <c r="E7" s="19" t="s">
         <v>8</v>
       </c>
@@ -1202,7 +1220,7 @@
       </c>
       <c r="B9" s="1">
         <f>IF(FPs!E19=0," ",FPs!E19)</f>
-        <v>180</v>
+        <v>196</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>13</v>
@@ -1232,7 +1250,7 @@
       </c>
       <c r="B11" s="1">
         <f>IF(OR(B9=" ",B10=" ")," ",B9*B10)</f>
-        <v>153.00000000000003</v>
+        <v>166.60000000000002</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>18</v>
@@ -1244,7 +1262,7 @@
       </c>
       <c r="B12" s="1">
         <f>B11*F8</f>
-        <v>3060.0000000000005</v>
+        <v>3332.0000000000005</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>20</v>
@@ -1256,7 +1274,7 @@
       </c>
       <c r="B13" s="1">
         <f>B11/(1/F9)</f>
-        <v>765.00000000000011</v>
+        <v>833.00000000000011</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>21</v>
@@ -1293,46 +1311,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="40"/>
+      <c r="G1" s="40"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="37"/>
-      <c r="B2" s="37"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
+      <c r="A2" s="41"/>
+      <c r="B2" s="41"/>
+      <c r="C2" s="41"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="41"/>
+      <c r="F2" s="41"/>
+      <c r="G2" s="41"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="35" t="s">
+      <c r="A3" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="34" t="s">
+      <c r="B3" s="38" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="34" t="s">
+      <c r="C3" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="D3" s="33" t="s">
+      <c r="D3" s="37" t="s">
         <v>26</v>
       </c>
-      <c r="E3" s="33"/>
-      <c r="F3" s="33"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="37"/>
       <c r="G3" s="6"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="35"/>
-      <c r="B4" s="34"/>
-      <c r="C4" s="34"/>
+      <c r="A4" s="39"/>
+      <c r="B4" s="38"/>
+      <c r="C4" s="38"/>
       <c r="D4" s="4" t="s">
         <v>27</v>
       </c>
@@ -1962,10 +1980,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1980,53 +1998,53 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="42" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
-      <c r="E1" s="52"/>
-      <c r="F1" s="52"/>
-      <c r="G1" s="52"/>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="53"/>
-      <c r="B2" s="53"/>
-      <c r="C2" s="53"/>
-      <c r="D2" s="53"/>
-      <c r="E2" s="53"/>
-      <c r="F2" s="53"/>
-      <c r="G2" s="53"/>
+      <c r="A2" s="43"/>
+      <c r="B2" s="43"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="43"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="34" t="s">
+      <c r="A3" s="38" t="s">
         <v>44</v>
       </c>
-      <c r="B3" s="34" t="s">
+      <c r="B3" s="38" t="s">
         <v>45</v>
       </c>
-      <c r="C3" s="34" t="s">
+      <c r="C3" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="D3" s="50" t="s">
+      <c r="D3" s="44" t="s">
         <v>26</v>
       </c>
-      <c r="E3" s="50"/>
-      <c r="F3" s="50"/>
+      <c r="E3" s="44"/>
+      <c r="F3" s="44"/>
       <c r="G3" s="21"/>
     </row>
-    <row r="4" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="34"/>
-      <c r="B4" s="34"/>
-      <c r="C4" s="34"/>
-      <c r="D4" s="51" t="s">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="38"/>
+      <c r="B4" s="38"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="E4" s="51" t="s">
+      <c r="E4" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="F4" s="51" t="s">
+      <c r="F4" s="24" t="s">
         <v>29</v>
       </c>
       <c r="G4" s="21" t="s">
@@ -2043,15 +2061,15 @@
       <c r="C5" s="3">
         <v>0</v>
       </c>
-      <c r="D5" s="54">
+      <c r="D5" s="25">
         <f>IF(AND(ISNUMBER($B5),ISNUMBER($C5)),IF(OR(AND($B5&lt;=19,$C5&lt;=1),AND($B5&lt;=5,$C5&lt;=3)),1,0)," ")</f>
         <v>1</v>
       </c>
-      <c r="E5" s="54">
+      <c r="E5" s="25">
         <f>IF(AND(ISNUMBER($B5),ISNUMBER($C5)),IF(OR(AND($B5&gt;19,$C5&lt;=1),AND($B5&gt;5,$B5&lt;=19,$C5&gt;1,$C5&lt;=3),AND($B5&lt;=5,$C5&gt;3)),1,0)," ")</f>
         <v>0</v>
       </c>
-      <c r="F5" s="54">
+      <c r="F5" s="25">
         <f>IF(AND(ISNUMBER($B5),ISNUMBER($C5)),IF(OR(AND($B5&gt;5,$C5&gt;3),AND($B5&gt;19,$C5&gt;1)),1,0)," ")</f>
         <v>0</v>
       </c>
@@ -2069,16 +2087,16 @@
       <c r="C6" s="3">
         <v>0</v>
       </c>
-      <c r="D6" s="54">
-        <f t="shared" ref="D6:D16" si="0">IF(AND(ISNUMBER($B6),ISNUMBER($C6)),IF(OR(AND($B6&lt;=19,$C6&lt;=1),AND($B6&lt;=5,$C6&lt;=3)),1,0)," ")</f>
-        <v>1</v>
-      </c>
-      <c r="E6" s="54">
-        <f t="shared" ref="E6:E16" si="1">IF(AND(ISNUMBER($B6),ISNUMBER($C6)),IF(OR(AND($B6&gt;19,$C6&lt;=1),AND($B6&gt;5,$B6&lt;=19,$C6&gt;1,$C6&lt;=3),AND($B6&lt;=5,$C6&gt;3)),1,0)," ")</f>
-        <v>0</v>
-      </c>
-      <c r="F6" s="54">
-        <f t="shared" ref="F6:F16" si="2">IF(AND(ISNUMBER($B6),ISNUMBER($C6)),IF(OR(AND($B6&gt;5,$C6&gt;3),AND($B6&gt;19,$C6&gt;1)),1,0)," ")</f>
+      <c r="D6" s="25">
+        <f t="shared" ref="D6:D20" si="0">IF(AND(ISNUMBER($B6),ISNUMBER($C6)),IF(OR(AND($B6&lt;=19,$C6&lt;=1),AND($B6&lt;=5,$C6&lt;=3)),1,0)," ")</f>
+        <v>1</v>
+      </c>
+      <c r="E6" s="25">
+        <f t="shared" ref="E6:E20" si="1">IF(AND(ISNUMBER($B6),ISNUMBER($C6)),IF(OR(AND($B6&gt;19,$C6&lt;=1),AND($B6&gt;5,$B6&lt;=19,$C6&gt;1,$C6&lt;=3),AND($B6&lt;=5,$C6&gt;3)),1,0)," ")</f>
+        <v>0</v>
+      </c>
+      <c r="F6" s="25">
+        <f t="shared" ref="F6:F20" si="2">IF(AND(ISNUMBER($B6),ISNUMBER($C6)),IF(OR(AND($B6&gt;5,$C6&gt;3),AND($B6&gt;19,$C6&gt;1)),1,0)," ")</f>
         <v>0</v>
       </c>
       <c r="G6" s="3" t="s">
@@ -2095,15 +2113,15 @@
       <c r="C7" s="3">
         <v>0</v>
       </c>
-      <c r="D7" s="54">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E7" s="54">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F7" s="54">
+      <c r="D7" s="25">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E7" s="25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F7" s="25">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -2121,15 +2139,15 @@
       <c r="C8" s="3">
         <v>0</v>
       </c>
-      <c r="D8" s="54">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E8" s="54">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F8" s="54">
+      <c r="D8" s="25">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E8" s="25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F8" s="25">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -2147,15 +2165,15 @@
       <c r="C9" s="3">
         <v>0</v>
       </c>
-      <c r="D9" s="54">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E9" s="54">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F9" s="54">
+      <c r="D9" s="25">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E9" s="25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F9" s="25">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -2173,15 +2191,15 @@
       <c r="C10" s="3">
         <v>0</v>
       </c>
-      <c r="D10" s="54">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E10" s="54">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F10" s="54">
+      <c r="D10" s="25">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E10" s="25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F10" s="25">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -2199,15 +2217,15 @@
       <c r="C11" s="3">
         <v>0</v>
       </c>
-      <c r="D11" s="54">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E11" s="54">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F11" s="54">
+      <c r="D11" s="25">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E11" s="25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F11" s="25">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -2225,15 +2243,15 @@
       <c r="C12" s="3">
         <v>1</v>
       </c>
-      <c r="D12" s="54">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E12" s="54">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F12" s="54">
+      <c r="D12" s="25">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E12" s="25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F12" s="25">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -2251,15 +2269,15 @@
       <c r="C13" s="3">
         <v>1</v>
       </c>
-      <c r="D13" s="54">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E13" s="54">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F13" s="54">
+      <c r="D13" s="25">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E13" s="25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F13" s="25">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -2277,15 +2295,15 @@
       <c r="C14" s="3">
         <v>1</v>
       </c>
-      <c r="D14" s="54">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E14" s="54">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F14" s="54">
+      <c r="D14" s="25">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E14" s="25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F14" s="25">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -2303,16 +2321,16 @@
       <c r="C15" s="3">
         <v>1</v>
       </c>
-      <c r="D15" s="54">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E15" s="54">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F15" s="54">
-        <f t="shared" si="2"/>
+      <c r="D15" s="25">
+        <f>IF(AND(ISNUMBER($B15),ISNUMBER($C15)),IF(OR(AND($B15&lt;=19,$C15&lt;=1),AND($B15&lt;=5,$C15&lt;=3)),1,0)," ")</f>
+        <v>1</v>
+      </c>
+      <c r="E15" s="25">
+        <f>IF(AND(ISNUMBER($B15),ISNUMBER($C15)),IF(OR(AND($B15&gt;19,$C15&lt;=1),AND($B15&gt;5,$B15&lt;=19,$C15&gt;1,$C15&lt;=3),AND($B15&lt;=5,$C15&gt;3)),1,0)," ")</f>
+        <v>0</v>
+      </c>
+      <c r="F15" s="25">
+        <f>IF(AND(ISNUMBER($B15),ISNUMBER($C15)),IF(OR(AND($B15&gt;5,$C15&gt;3),AND($B15&gt;19,$C15&gt;1)),1,0)," ")</f>
         <v>0</v>
       </c>
       <c r="G15" s="3" t="s">
@@ -2320,42 +2338,137 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="3"/>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="54" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="E16" s="54" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="F16" s="54" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="G16" s="3"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="B16" s="3">
+        <v>1</v>
+      </c>
+      <c r="C16" s="3">
+        <v>1</v>
+      </c>
+      <c r="D16" s="25">
+        <f>IF(AND(ISNUMBER($B16),ISNUMBER($C16)),IF(OR(AND($B16&lt;=19,$C16&lt;=1),AND($B16&lt;=5,$C16&lt;=3)),1,0)," ")</f>
+        <v>1</v>
+      </c>
+      <c r="E16" s="25">
+        <f>IF(AND(ISNUMBER($B16),ISNUMBER($C16)),IF(OR(AND($B16&gt;19,$C16&lt;=1),AND($B16&gt;5,$B16&lt;=19,$C16&gt;1,$C16&lt;=3),AND($B16&lt;=5,$C16&gt;3)),1,0)," ")</f>
+        <v>0</v>
+      </c>
+      <c r="F16" s="25">
+        <f>IF(AND(ISNUMBER($B16),ISNUMBER($C16)),IF(OR(AND($B16&gt;5,$C16&gt;3),AND($B16&gt;19,$C16&gt;1)),1,0)," ")</f>
+        <v>0</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="B17" s="3">
+        <v>4</v>
+      </c>
+      <c r="C17" s="3">
+        <v>1</v>
+      </c>
+      <c r="D17" s="25">
+        <f>IF(AND(ISNUMBER($B17),ISNUMBER($C17)),IF(OR(AND($B17&lt;=19,$C17&lt;=1),AND($B17&lt;=5,$C17&lt;=3)),1,0)," ")</f>
+        <v>1</v>
+      </c>
+      <c r="E17" s="25">
+        <f>IF(AND(ISNUMBER($B17),ISNUMBER($C17)),IF(OR(AND($B17&gt;19,$C17&lt;=1),AND($B17&gt;5,$B17&lt;=19,$C17&gt;1,$C17&lt;=3),AND($B17&lt;=5,$C17&gt;3)),1,0)," ")</f>
+        <v>0</v>
+      </c>
+      <c r="F17" s="25">
+        <f>IF(AND(ISNUMBER($B17),ISNUMBER($C17)),IF(OR(AND($B17&gt;5,$C17&gt;3),AND($B17&gt;19,$C17&gt;1)),1,0)," ")</f>
+        <v>0</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="B18" s="3">
+        <v>4</v>
+      </c>
+      <c r="C18" s="3">
+        <v>1</v>
+      </c>
+      <c r="D18" s="25">
+        <f>IF(AND(ISNUMBER($B18),ISNUMBER($C18)),IF(OR(AND($B18&lt;=19,$C18&lt;=1),AND($B18&lt;=5,$C18&lt;=3)),1,0)," ")</f>
+        <v>1</v>
+      </c>
+      <c r="E18" s="25">
+        <f>IF(AND(ISNUMBER($B18),ISNUMBER($C18)),IF(OR(AND($B18&gt;19,$C18&lt;=1),AND($B18&gt;5,$B18&lt;=19,$C18&gt;1,$C18&lt;=3),AND($B18&lt;=5,$C18&gt;3)),1,0)," ")</f>
+        <v>0</v>
+      </c>
+      <c r="F18" s="25">
+        <f>IF(AND(ISNUMBER($B18),ISNUMBER($C18)),IF(OR(AND($B18&gt;5,$C18&gt;3),AND($B18&gt;19,$C18&gt;1)),1,0)," ")</f>
+        <v>0</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="B19" s="3">
+        <v>4</v>
+      </c>
+      <c r="C19" s="3">
+        <v>1</v>
+      </c>
+      <c r="D19" s="25">
+        <f>IF(AND(ISNUMBER($B19),ISNUMBER($C19)),IF(OR(AND($B19&lt;=19,$C19&lt;=1),AND($B19&lt;=5,$C19&lt;=3)),1,0)," ")</f>
+        <v>1</v>
+      </c>
+      <c r="E19" s="25">
+        <f>IF(AND(ISNUMBER($B19),ISNUMBER($C19)),IF(OR(AND($B19&gt;19,$C19&lt;=1),AND($B19&gt;5,$B19&lt;=19,$C19&gt;1,$C19&lt;=3),AND($B19&lt;=5,$C19&gt;3)),1,0)," ")</f>
+        <v>0</v>
+      </c>
+      <c r="F19" s="25">
+        <f>IF(AND(ISNUMBER($B19),ISNUMBER($C19)),IF(OR(AND($B19&gt;5,$C19&gt;3),AND($B19&gt;19,$C19&gt;1)),1,0)," ")</f>
+        <v>0</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="3"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="25"/>
+      <c r="E20" s="25"/>
+      <c r="F20" s="25"/>
+      <c r="G20" s="3"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="54">
-        <f>SUM(D5:D16)</f>
-        <v>11</v>
-      </c>
-      <c r="E17" s="54">
-        <f t="shared" ref="E17:F17" si="3">SUM(E5:E16)</f>
-        <v>0</v>
-      </c>
-      <c r="F17" s="54">
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="25">
+        <f>SUM(D5:D20)</f>
+        <v>15</v>
+      </c>
+      <c r="E21" s="25">
+        <f t="shared" ref="E21:F21" si="3">SUM(E5:E20)</f>
+        <v>0</v>
+      </c>
+      <c r="F21" s="25">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="G17" s="3"/>
+      <c r="G21" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -2390,63 +2503,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="40" t="s">
         <v>51</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36"/>
-      <c r="I1" s="36"/>
-      <c r="J1" s="36"/>
-      <c r="K1" s="36"/>
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="40"/>
+      <c r="G1" s="40"/>
+      <c r="H1" s="40"/>
+      <c r="I1" s="40"/>
+      <c r="J1" s="40"/>
+      <c r="K1" s="40"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="37"/>
-      <c r="B2" s="37"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="37"/>
-      <c r="K2" s="37"/>
+      <c r="A2" s="41"/>
+      <c r="B2" s="41"/>
+      <c r="C2" s="41"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="41"/>
+      <c r="F2" s="41"/>
+      <c r="G2" s="41"/>
+      <c r="H2" s="41"/>
+      <c r="I2" s="41"/>
+      <c r="J2" s="41"/>
+      <c r="K2" s="41"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="34" t="s">
+      <c r="A3" s="38" t="s">
         <v>52</v>
       </c>
-      <c r="B3" s="38" t="s">
+      <c r="B3" s="45" t="s">
         <v>53</v>
       </c>
-      <c r="C3" s="39"/>
-      <c r="D3" s="48"/>
-      <c r="E3" s="38" t="s">
+      <c r="C3" s="46"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="45" t="s">
         <v>54</v>
       </c>
-      <c r="F3" s="39"/>
-      <c r="G3" s="49"/>
-      <c r="H3" s="50" t="s">
+      <c r="F3" s="46"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="44" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="50"/>
-      <c r="J3" s="50"/>
+      <c r="I3" s="44"/>
+      <c r="J3" s="44"/>
       <c r="K3" s="21"/>
     </row>
     <row r="4" spans="1:11" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="34"/>
+      <c r="A4" s="38"/>
       <c r="B4" s="7" t="s">
         <v>24</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="51" t="s">
+      <c r="D4" s="24" t="s">
         <v>26</v>
       </c>
       <c r="E4" s="7" t="s">
@@ -2455,16 +2568,16 @@
       <c r="F4" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="G4" s="51" t="s">
+      <c r="G4" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="H4" s="51" t="s">
+      <c r="H4" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="I4" s="51" t="s">
+      <c r="I4" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="J4" s="51" t="s">
+      <c r="J4" s="24" t="s">
         <v>29</v>
       </c>
       <c r="K4" s="21" t="s">
@@ -2887,46 +3000,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="40" t="s">
         <v>57</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="40"/>
+      <c r="G1" s="40"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="37"/>
-      <c r="B2" s="37"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
+      <c r="A2" s="41"/>
+      <c r="B2" s="41"/>
+      <c r="C2" s="41"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="41"/>
+      <c r="F2" s="41"/>
+      <c r="G2" s="41"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="35" t="s">
+      <c r="A3" s="39" t="s">
         <v>58</v>
       </c>
-      <c r="B3" s="35" t="s">
+      <c r="B3" s="39" t="s">
         <v>55</v>
       </c>
-      <c r="C3" s="35" t="s">
+      <c r="C3" s="39" t="s">
         <v>59</v>
       </c>
-      <c r="D3" s="33" t="s">
+      <c r="D3" s="37" t="s">
         <v>26</v>
       </c>
-      <c r="E3" s="33"/>
-      <c r="F3" s="33"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="37"/>
       <c r="G3" s="6"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="35"/>
-      <c r="B4" s="35"/>
-      <c r="C4" s="35"/>
+      <c r="A4" s="39"/>
+      <c r="B4" s="39"/>
+      <c r="C4" s="39"/>
       <c r="D4" s="4" t="s">
         <v>27</v>
       </c>
@@ -3277,46 +3390,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="40" t="s">
         <v>68</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="40"/>
+      <c r="G1" s="40"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="37"/>
-      <c r="B2" s="37"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
+      <c r="A2" s="41"/>
+      <c r="B2" s="41"/>
+      <c r="C2" s="41"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="41"/>
+      <c r="F2" s="41"/>
+      <c r="G2" s="41"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="35" t="s">
+      <c r="A3" s="39" t="s">
         <v>58</v>
       </c>
-      <c r="B3" s="34" t="s">
+      <c r="B3" s="38" t="s">
         <v>55</v>
       </c>
-      <c r="C3" s="34" t="s">
+      <c r="C3" s="38" t="s">
         <v>59</v>
       </c>
-      <c r="D3" s="33" t="s">
+      <c r="D3" s="37" t="s">
         <v>26</v>
       </c>
-      <c r="E3" s="33"/>
-      <c r="F3" s="33"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="37"/>
       <c r="G3" s="6"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="35"/>
-      <c r="B4" s="34"/>
-      <c r="C4" s="34"/>
+      <c r="A4" s="39"/>
+      <c r="B4" s="38"/>
+      <c r="C4" s="38"/>
       <c r="D4" s="4" t="s">
         <v>27</v>
       </c>
@@ -3596,20 +3709,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="47" t="s">
         <v>69</v>
       </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40"/>
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="41"/>
-      <c r="B2" s="41"/>
-      <c r="C2" s="41"/>
-      <c r="D2" s="41"/>
-      <c r="E2" s="41"/>
+      <c r="A2" s="48"/>
+      <c r="B2" s="48"/>
+      <c r="C2" s="48"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="48"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
@@ -3629,7 +3742,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="43" t="s">
+      <c r="A4" s="50" t="s">
         <v>75</v>
       </c>
       <c r="B4" s="10" t="s">
@@ -3648,7 +3761,7 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="44"/>
+      <c r="A5" s="51"/>
       <c r="B5" s="10" t="s">
         <v>28</v>
       </c>
@@ -3665,7 +3778,7 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="45"/>
+      <c r="A6" s="52"/>
       <c r="B6" s="10" t="s">
         <v>29</v>
       </c>
@@ -3682,7 +3795,7 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="43" t="s">
+      <c r="A7" s="50" t="s">
         <v>76</v>
       </c>
       <c r="B7" s="10" t="s">
@@ -3701,7 +3814,7 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="44"/>
+      <c r="A8" s="51"/>
       <c r="B8" s="10" t="s">
         <v>28</v>
       </c>
@@ -3718,7 +3831,7 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="45"/>
+      <c r="A9" s="52"/>
       <c r="B9" s="10" t="s">
         <v>29</v>
       </c>
@@ -3735,7 +3848,7 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="43" t="s">
+      <c r="A10" s="50" t="s">
         <v>77</v>
       </c>
       <c r="B10" s="10" t="s">
@@ -3754,7 +3867,7 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="44"/>
+      <c r="A11" s="51"/>
       <c r="B11" s="10" t="s">
         <v>28</v>
       </c>
@@ -3771,7 +3884,7 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="45"/>
+      <c r="A12" s="52"/>
       <c r="B12" s="10" t="s">
         <v>29</v>
       </c>
@@ -3788,31 +3901,31 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="43" t="s">
+      <c r="A13" s="50" t="s">
         <v>78</v>
       </c>
       <c r="B13" s="10" t="s">
         <v>27</v>
       </c>
       <c r="C13" s="1">
-        <f>EOs!$D$17</f>
-        <v>11</v>
+        <f>EOs!$D$21</f>
+        <v>15</v>
       </c>
       <c r="D13" s="1">
         <v>4</v>
       </c>
       <c r="E13" s="1">
         <f t="shared" si="0"/>
-        <v>44</v>
+        <v>60</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="44"/>
+      <c r="A14" s="51"/>
       <c r="B14" s="10" t="s">
         <v>28</v>
       </c>
       <c r="C14" s="1">
-        <f>EOs!$E$17</f>
+        <f>EOs!$E$21</f>
         <v>0</v>
       </c>
       <c r="D14" s="1">
@@ -3824,12 +3937,12 @@
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="45"/>
+      <c r="A15" s="52"/>
       <c r="B15" s="10" t="s">
         <v>29</v>
       </c>
       <c r="C15" s="1">
-        <f>EOs!$F$17</f>
+        <f>EOs!$F$21</f>
         <v>0</v>
       </c>
       <c r="D15" s="1">
@@ -3841,7 +3954,7 @@
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="43" t="s">
+      <c r="A16" s="50" t="s">
         <v>79</v>
       </c>
       <c r="B16" s="10" t="s">
@@ -3860,7 +3973,7 @@
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="44"/>
+      <c r="A17" s="51"/>
       <c r="B17" s="10" t="s">
         <v>28</v>
       </c>
@@ -3877,7 +3990,7 @@
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="45"/>
+      <c r="A18" s="52"/>
       <c r="B18" s="10" t="s">
         <v>29</v>
       </c>
@@ -3894,15 +4007,15 @@
       </c>
     </row>
     <row r="19" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="42" t="s">
+      <c r="A19" s="49" t="s">
         <v>80</v>
       </c>
-      <c r="B19" s="42"/>
-      <c r="C19" s="42"/>
-      <c r="D19" s="42"/>
+      <c r="B19" s="49"/>
+      <c r="C19" s="49"/>
+      <c r="D19" s="49"/>
       <c r="E19" s="1">
         <f>SUM(E4:E18)</f>
-        <v>180</v>
+        <v>196</v>
       </c>
     </row>
   </sheetData>
@@ -3936,24 +4049,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="53" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
+      <c r="B1" s="53"/>
+      <c r="C1" s="53"/>
+      <c r="D1" s="53"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="46"/>
-      <c r="B2" s="46"/>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
+      <c r="A2" s="53"/>
+      <c r="B2" s="53"/>
+      <c r="C2" s="53"/>
+      <c r="D2" s="53"/>
     </row>
     <row r="3" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="23" t="s">
+      <c r="A3" s="26" t="s">
         <v>81</v>
       </c>
-      <c r="B3" s="23"/>
+      <c r="B3" s="26"/>
       <c r="C3" s="9" t="s">
         <v>82</v>
       </c>
@@ -4158,10 +4271,10 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="47" t="s">
+      <c r="A18" s="54" t="s">
         <v>97</v>
       </c>
-      <c r="B18" s="47"/>
+      <c r="B18" s="54"/>
       <c r="C18" s="3">
         <f>IF(AND(ISNUMBER(C4),ISNUMBER(C5),ISNUMBER(C6),ISNUMBER(C7),ISNUMBER(C8),ISNUMBER(C9),ISNUMBER(C10),ISNUMBER(C11),ISNUMBER(C12),ISNUMBER(C13),ISNUMBER(C14),ISNUMBER(C15),ISNUMBER(C16),ISNUMBER(C17)),SUM(C4:C17)," ")</f>
         <v>20</v>
@@ -4171,10 +4284,10 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="47" t="s">
+      <c r="A19" s="54" t="s">
         <v>15</v>
       </c>
-      <c r="B19" s="47"/>
+      <c r="B19" s="54"/>
       <c r="C19" s="3">
         <f>IF(OR($C18=" ",C4&gt;5,C5&gt;5,C6&gt;5,C7&gt;5,C8&gt;5,C9&gt;8,C10&gt;5,C11&gt;5,C12&gt;5,C13&gt;5,C14&gt;5,C15&gt;5,C16&gt;5,C17&gt;5)," ",(C18*0.01)+0.65)</f>
         <v>0.85000000000000009</v>

</xml_diff>